<commit_message>
Added temp file management & highlight element
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>KeyWord</t>
   </si>
@@ -49,13 +49,55 @@
     <t>CheckBoxText</t>
   </si>
   <si>
-    <t>TestCase1_validateCheckBox</t>
-  </si>
-  <si>
     <t>Validate checkboxes</t>
   </si>
   <si>
     <t>kw_checkboxes</t>
+  </si>
+  <si>
+    <t>TestCase3_validateCheckBox</t>
+  </si>
+  <si>
+    <t>TestCase4_validateRadioButton</t>
+  </si>
+  <si>
+    <t>Validate Radio Buttons</t>
+  </si>
+  <si>
+    <t>kw_radiobuttons</t>
+  </si>
+  <si>
+    <t>OptionFromList</t>
+  </si>
+  <si>
+    <t>Select Dropdown List</t>
+  </si>
+  <si>
+    <t>Check Box Demo</t>
+  </si>
+  <si>
+    <t>Radio Buttons Demo</t>
+  </si>
+  <si>
+    <t>TestCase5_validateRadioButton</t>
+  </si>
+  <si>
+    <t>Validate Drop Down Lists</t>
+  </si>
+  <si>
+    <t>kw_ddlist</t>
+  </si>
+  <si>
+    <t>FirstOption</t>
+  </si>
+  <si>
+    <t>SecondOption</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Florida#New Jersey#Texas#Washington</t>
   </si>
 </sst>
 </file>
@@ -423,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,9 +480,10 @@
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -462,8 +505,17 @@
       <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -481,16 +533,19 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -498,8 +553,58 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pop up blocker, download path, Assertion Manager. mentioned in README line 20, 21 & 22.
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>KeyWord</t>
   </si>
@@ -98,6 +98,45 @@
   </si>
   <si>
     <t>Florida#New Jersey#Texas#Washington</t>
+  </si>
+  <si>
+    <t>TestCase5_validateJSAlerts</t>
+  </si>
+  <si>
+    <t>kw_alerts</t>
+  </si>
+  <si>
+    <t>TestCase6_validateJSConfirmation</t>
+  </si>
+  <si>
+    <t>Validate JavaScript Alerts</t>
+  </si>
+  <si>
+    <t>Validate JavaScript Confirmations</t>
+  </si>
+  <si>
+    <t>kw_confirm</t>
+  </si>
+  <si>
+    <t>TestCase7_validateJSPrompt</t>
+  </si>
+  <si>
+    <t>Validate JavaScript Prompt</t>
+  </si>
+  <si>
+    <t>kw_prompt</t>
+  </si>
+  <si>
+    <t>AlertAction</t>
+  </si>
+  <si>
+    <t>accept</t>
+  </si>
+  <si>
+    <t>dismiss</t>
+  </si>
+  <si>
+    <t>Selenium</t>
   </si>
 </sst>
 </file>
@@ -465,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +519,10 @@
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -514,8 +553,11 @@
       <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -536,8 +578,9 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -558,8 +601,9 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -578,8 +622,9 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -602,6 +647,74 @@
       <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added line 23 in Pros and line 3 in Cons of README
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>KeyWord</t>
   </si>
@@ -137,6 +137,60 @@
   </si>
   <si>
     <t>Selenium</t>
+  </si>
+  <si>
+    <t>HardAssert</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TestCase8_validateSingleDatePickerBootStrap</t>
+  </si>
+  <si>
+    <t>Validate Single Date Picking BootStrap</t>
+  </si>
+  <si>
+    <t>kw_bootStrapDate</t>
+  </si>
+  <si>
+    <t>Bootstrap Date Picker</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>27/02/2021</t>
+  </si>
+  <si>
+    <t>Date pickers</t>
+  </si>
+  <si>
+    <t>TestCase9_validateDownloadTableData</t>
+  </si>
+  <si>
+    <t>Validate Download of Multiple Files from Web Table</t>
+  </si>
+  <si>
+    <t>kw_downloadtabledata</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Table Data Download</t>
+  </si>
+  <si>
+    <t>CSV#Excel#PDF</t>
+  </si>
+  <si>
+    <t>FileNames</t>
+  </si>
+  <si>
+    <t>Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.csv#Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.xlsx#Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.pdf</t>
   </si>
 </sst>
 </file>
@@ -193,13 +247,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,14 +572,16 @@
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -533,31 +592,40 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -567,20 +635,25 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1">
         <v>113</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>229</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -590,20 +663,25 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -613,18 +691,23 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -634,24 +717,31 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -661,18 +751,25 @@
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -682,18 +779,25 @@
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -703,17 +807,86 @@
       <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added line 24 & 25 in Readme.
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>KeyWord</t>
   </si>
@@ -191,6 +191,21 @@
   </si>
   <si>
     <t>Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.csv#Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.xlsx#Selenium Easy - Download Table Data to CSV, Excel, PDF and Print.pdf</t>
+  </si>
+  <si>
+    <t>TestCase10_validateFecthTableData</t>
+  </si>
+  <si>
+    <t>Validate different column values of different Candidates in the web table.</t>
+  </si>
+  <si>
+    <t>kw_fetchtabledata</t>
+  </si>
+  <si>
+    <t>Airi Satou#Bradley Greer#Brenden Wagner#Colleen Hurst</t>
+  </si>
+  <si>
+    <t>Position#Age#Salary</t>
   </si>
 </sst>
 </file>
@@ -561,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,6 +904,38 @@
         <v>58</v>
       </c>
     </row>
+    <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="N11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added line 26 in Readme
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>KeyWord</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Position#Age#Salary</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>#337ab7</t>
   </si>
 </sst>
 </file>
@@ -576,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +599,10 @@
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -639,8 +645,11 @@
       <c r="N1" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,8 +676,9 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -695,8 +705,9 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -721,8 +732,9 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -755,8 +767,9 @@
       <c r="N5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -783,8 +796,9 @@
       <c r="N6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -811,8 +825,9 @@
       <c r="N7" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -841,8 +856,9 @@
       <c r="N8" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -871,8 +887,9 @@
         <v>49</v>
       </c>
       <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -903,8 +920,11 @@
       <c r="N10" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="O10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -935,6 +955,7 @@
       <c r="N11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="O11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Con number 4 in Readme file
Signed-off-by: Dell <Dell@Dell-PC>
</commit_message>
<xml_diff>
--- a/TestData/DataSheet.xlsx
+++ b/TestData/DataSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>KeyWord</t>
   </si>
@@ -212,6 +212,21 @@
   </si>
   <si>
     <t>#337ab7</t>
+  </si>
+  <si>
+    <t>TestCase11_validateDragAndDrop</t>
+  </si>
+  <si>
+    <t>Validate Drag And Drop functionality.</t>
+  </si>
+  <si>
+    <t>kw_draganddrop</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Drag and Drop</t>
   </si>
 </sst>
 </file>
@@ -582,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="H11" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,6 +972,35 @@
       </c>
       <c r="O11" s="2"/>
     </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>